<commit_message>
print many works and subworks in excel
</commit_message>
<xml_diff>
--- a/public/reports/reporteRudelEmpty.xlsx
+++ b/public/reports/reporteRudelEmpty.xlsx
@@ -41,7 +41,7 @@
     <t>Supervisor turno día:</t>
   </si>
   <si>
-    <t>Ubicación del equipo: </t>
+    <t>Ubicación del equipo:</t>
   </si>
   <si>
     <t>Supervisores turno noche:</t>
@@ -160,6 +160,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -273,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,10 +308,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,8 +442,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7295918367347"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4234693877551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.8469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
@@ -498,7 +495,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -514,17 +511,17 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -533,7 +530,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -542,7 +539,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -551,16 +548,16 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -572,7 +569,7 @@
       <c r="E18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>26</v>
       </c>
     </row>
@@ -637,45 +634,45 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="11"/>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12" t="s">
+      <c r="D34" s="11"/>
+      <c r="E34" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="15"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>30</v>
       </c>
       <c r="F36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="13"/>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="12"/>
+      <c r="C38" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -687,13 +684,13 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="10"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="F40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -717,11 +714,11 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="20"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>